<commit_message>
correlaciones entre covariables, añadir desviación estandar a la tabla de descriptivas
</commit_message>
<xml_diff>
--- a/descriptivas.xlsx
+++ b/descriptivas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t xml:space="preserve"> Min.   1st Qu.     Median       Mean    3rd Qu.      Max.</t>
   </si>
@@ -159,6 +159,36 @@
   </si>
   <si>
     <t>-116.2</t>
+  </si>
+  <si>
+    <t>Desviación Est.</t>
+  </si>
+  <si>
+    <t>120509.8</t>
+  </si>
+  <si>
+    <t>1.735087</t>
+  </si>
+  <si>
+    <t>14.5956</t>
+  </si>
+  <si>
+    <t>1539.323</t>
+  </si>
+  <si>
+    <t>360.0191</t>
+  </si>
+  <si>
+    <t>779.5774</t>
+  </si>
+  <si>
+    <t>328.173</t>
+  </si>
+  <si>
+    <t>1.790967</t>
+  </si>
+  <si>
+    <t>2.099794</t>
   </si>
 </sst>
 </file>
@@ -228,13 +258,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -249,6 +276,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -534,7 +567,7 @@
   <dimension ref="C3:J26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,235 +576,265 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>32500</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>229600</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>294400</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>318400</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>419100</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>500000</v>
       </c>
+      <c r="J4" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>3697</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>3905</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>4554</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>15</v>
       </c>
+      <c r="J5" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>52</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>52</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>52</v>
       </c>
+      <c r="J6" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>52</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>1580</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>2218</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>2537</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>3166</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>12480</v>
       </c>
+      <c r="J7" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>13</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>346</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>506</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>2747</v>
       </c>
+      <c r="J8" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>55</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>836</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>1168</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>1303</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>1608</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>5640</v>
       </c>
+      <c r="J9" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>13</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>2538</v>
       </c>
+      <c r="J10" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="J11" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>44</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
@@ -827,5 +890,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="J5:J12" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
beamer full, cambio descriptivas y graficos de cajas
</commit_message>
<xml_diff>
--- a/descriptivas.xlsx
+++ b/descriptivas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve"> Min.   1st Qu.     Median       Mean    3rd Qu.      Max.</t>
   </si>
@@ -56,15 +56,6 @@
     <t>Longitud                -122.5000   -122.40   -122.400   -121.500   -122.400   -116.20</t>
   </si>
   <si>
-    <t>Valor medio de la casa</t>
-  </si>
-  <si>
-    <t>Ingreso medio</t>
-  </si>
-  <si>
-    <t>Edad media</t>
-  </si>
-  <si>
     <t>Total de habitaciones</t>
   </si>
   <si>
@@ -77,12 +68,6 @@
     <t>Hogares</t>
   </si>
   <si>
-    <t>Latitud</t>
-  </si>
-  <si>
-    <t>Longitud</t>
-  </si>
-  <si>
     <t>Min.</t>
   </si>
   <si>
@@ -113,12 +98,6 @@
     <t xml:space="preserve">327.80   </t>
   </si>
   <si>
-    <t xml:space="preserve">37.72     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 37.81</t>
-  </si>
-  <si>
     <t>42.2</t>
   </si>
   <si>
@@ -137,30 +116,6 @@
     <t>664.5</t>
   </si>
   <si>
-    <t>32.61</t>
-  </si>
-  <si>
-    <t>37.75</t>
-  </si>
-  <si>
-    <t>36.95</t>
-  </si>
-  <si>
-    <t>37.78</t>
-  </si>
-  <si>
-    <t>-122.5</t>
-  </si>
-  <si>
-    <t>-122.4</t>
-  </si>
-  <si>
-    <t>-121.5</t>
-  </si>
-  <si>
-    <t>-116.2</t>
-  </si>
-  <si>
     <t>Desviación Est.</t>
   </si>
   <si>
@@ -185,10 +140,13 @@
     <t>328.173</t>
   </si>
   <si>
-    <t>1.790967</t>
-  </si>
-  <si>
-    <t>2.099794</t>
+    <t>Edad mediana</t>
+  </si>
+  <si>
+    <t>Valor mediano de las viviendas</t>
+  </si>
+  <si>
+    <t>Ingreso mediano</t>
   </si>
 </sst>
 </file>
@@ -258,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -271,9 +229,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -564,15 +519,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J26"/>
+  <dimension ref="C3:J24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -580,32 +535,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="7"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>45</v>
+      <c r="J3" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3">
         <v>32500</v>
@@ -625,19 +580,19 @@
       <c r="I4" s="3">
         <v>500000</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>46</v>
+      <c r="J4" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4">
         <v>3697</v>
@@ -652,24 +607,24 @@
         <v>15</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3">
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3">
         <v>52</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H6" s="3">
         <v>52</v>
@@ -678,12 +633,12 @@
         <v>52</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3">
         <v>52</v>
@@ -704,12 +659,12 @@
         <v>12480</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3">
         <v>13</v>
@@ -721,21 +676,21 @@
         <v>506</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I8" s="3">
         <v>2747</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3">
         <v>55</v>
@@ -756,134 +711,82 @@
         <v>5640</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="9">
+        <v>13</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="3">
+      <c r="H10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="9">
         <v>2538</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="J10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>54</v>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -891,7 +794,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J5:J12" numberStoredAsText="1"/>
+    <ignoredError sqref="J5:J10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final de los finales
</commit_message>
<xml_diff>
--- a/descriptivas.xlsx
+++ b/descriptivas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve"> Min.   1st Qu.     Median       Mean    3rd Qu.      Max.</t>
   </si>
@@ -147,13 +147,140 @@
   </si>
   <si>
     <t>Ingreso mediano</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ingreso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">       1.00000000  0.01725444   0.07902878  -0.1813679 -0.1625779 -0.1604979</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hogares</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">      -0.16049785 -0.14456632   0.86527649   0.9887048  0.8539180  1.0000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Edad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">         0.01725444  1.00000000  -0.31169821  -0.1702448 -0.2651765 -0.1445663</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Habitaciones</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">   0.07902878 -0.31169821   1.00000000   0.8620727  0.8576863  0.8652765</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dormitorios       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>-0.18136789 -0.17024480   0.86207267   1.0000000  0.8340611  0.9887048</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                                         Ingreso                   Edad                 Habitaciones        Dormitorios      Población          Hogares</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Población</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">    -0.16257787 -0.26517653   0.85768626   0.8340611  1.0000000  0.8539180</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +301,14 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -238,6 +373,18 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,15 +666,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J24"/>
+  <dimension ref="C3:J34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="96.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -790,6 +937,41 @@
         <v>9</v>
       </c>
     </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>